<commit_message>
Back log of commits to changes in codes and generation of figures - will clean in the next day or so to organize the repository
Code and data describe size spectra analysis of zooplankton and macroinvertebrate data in seven shallow lakes in northwestern Iowa
</commit_message>
<xml_diff>
--- a/MIV Biomass Equations.xlsx
+++ b/MIV Biomass Equations.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Box Sync\Butts_Scripts\Carp Lakes\carp-foodweb-change\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tjbut\Box Sync\Butts_Scripts\Carp Lakes\carp-foodweb-change\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AA2237-D24E-490F-9A61-9EC8CB322BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293B7679-B274-4386-9EB3-C2BB5CB7B73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{5A58281E-6832-4FEA-9FDA-DF4A7482EADD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5A58281E-6832-4FEA-9FDA-DF4A7482EADD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Averages from Benke" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Averages from Benke" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="85">
   <si>
     <t>taxa</t>
   </si>
@@ -123,41 +124,9 @@
     <t xml:space="preserve">Notes </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Based off </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Planorbella (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Planorbidae) pulmonate snails with planispiral shells </t>
-    </r>
-  </si>
-  <si>
-    <t>ln(dry mass) = 1.72*(SL) + 0.8*(AW) - 9.49</t>
-  </si>
-  <si>
     <t>units</t>
   </si>
   <si>
-    <t>g, mm</t>
-  </si>
-  <si>
     <t>SL</t>
   </si>
   <si>
@@ -186,9 +155,6 @@
   </si>
   <si>
     <t>citation</t>
-  </si>
-  <si>
-    <t>Obaza &amp; Ruehl 2013</t>
   </si>
   <si>
     <t>Benke et al. 1999</t>
@@ -376,12 +342,21 @@
   <si>
     <t>Dry mass = 0.04736 + BL^3</t>
   </si>
+  <si>
+    <t xml:space="preserve">General Planorbidae equation </t>
+  </si>
+  <si>
+    <t>Methot et al. 2012</t>
+  </si>
+  <si>
+    <t>log10(DM) = -1.12 + 2.90*[log10(SL)]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,6 +396,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -467,9 +449,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF886B5-3827-4BE8-9F82-95F9F0AC3E48}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -814,10 +794,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
         <v>27</v>
@@ -827,143 +807,143 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>42</v>
+      <c r="B2" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="10"/>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="10"/>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>72</v>
+      <c r="B5" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>36</v>
+        <v>69</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
+      <c r="G5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
+      <c r="B6" s="3"/>
       <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="10"/>
+        <v>30</v>
+      </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
+      <c r="B7" s="3"/>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -971,19 +951,19 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -991,19 +971,19 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1011,19 +991,19 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1031,19 +1011,19 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1051,19 +1031,19 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1071,19 +1051,19 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1091,19 +1071,19 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1111,7 +1091,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1119,22 +1099,22 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1142,17 +1122,17 @@
         <v>15</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1160,19 +1140,19 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1180,19 +1160,19 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1200,22 +1180,22 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" t="s">
         <v>43</v>
-      </c>
-      <c r="C21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1223,19 +1203,19 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1243,17 +1223,17 @@
         <v>20</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1261,19 +1241,19 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1281,22 +1261,22 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1304,19 +1284,19 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1324,12 +1304,12 @@
         <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1337,19 +1317,19 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1357,31 +1337,25 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="G2:N4"/>
-    <mergeCell ref="G5:N7"/>
-    <mergeCell ref="D3:D4"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1389,6 +1363,641 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF29F30D-F75C-47FA-8783-CB61C43CE5B9}">
+  <dimension ref="A1:N36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+    </row>
+    <row r="27" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27" s="3"/>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="10"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N42">
+    <sortCondition ref="B2:B42"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DCA1C7B-53BA-4E2E-A47F-3493F1FD4251}">
   <dimension ref="B2:L41"/>
   <sheetViews>
@@ -1400,33 +2009,33 @@
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="L3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -1880,7 +2489,7 @@
         <v>2.3580000000000001</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G33">
         <f>AVERAGE(G4:G31)</f>
@@ -1941,7 +2550,7 @@
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C41">
         <f>AVERAGE(C4:C39)</f>

</xml_diff>